<commit_message>
feat(FileController): agregar método para validar archivos y mejorar manejo de solicitudes
</commit_message>
<xml_diff>
--- a/storage/templates/import/bulk-data/plantilla-docente.xlsx
+++ b/storage/templates/import/bulk-data/plantilla-docente.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Projects\PyEduVirtual\PyEducaVirtualBackend\storage\templates\import\bulk-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9FDA96-DF5A-491C-9995-E65A6E85470A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096F91CF-28AF-4B04-A8D4-F3FD3E482E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
   <si>
     <t>DNI</t>
   </si>
@@ -53,12 +54,6 @@
     <t>Sexo</t>
   </si>
   <si>
-    <t>Categoria</t>
-  </si>
-  <si>
-    <t>Condicion</t>
-  </si>
-  <si>
     <t>Correo Institucional</t>
   </si>
   <si>
@@ -81,6 +76,90 @@
   </si>
   <si>
     <t>Horas laborales</t>
+  </si>
+  <si>
+    <t>AGIPS</t>
+  </si>
+  <si>
+    <t>RUBIO</t>
+  </si>
+  <si>
+    <t>RICARDO GERMAN</t>
+  </si>
+  <si>
+    <t>v_cDocenteDireccion</t>
+  </si>
+  <si>
+    <t>cPersDocumento</t>
+  </si>
+  <si>
+    <t>cPersPaterno</t>
+  </si>
+  <si>
+    <t>v_cPersPaterno</t>
+  </si>
+  <si>
+    <t>cPersMaterno</t>
+  </si>
+  <si>
+    <t>v_cPersMaterno</t>
+  </si>
+  <si>
+    <t>cPersNombre</t>
+  </si>
+  <si>
+    <t>v_cPersNombre</t>
+  </si>
+  <si>
+    <t>cPersSexo</t>
+  </si>
+  <si>
+    <t>v_cPersSexo</t>
+  </si>
+  <si>
+    <t>cDocenteCorreoInstitucional</t>
+  </si>
+  <si>
+    <t>v_cDocenteCorreoInstitucional</t>
+  </si>
+  <si>
+    <t>cDocenteCorreo</t>
+  </si>
+  <si>
+    <t>v_cDocenteCorreo</t>
+  </si>
+  <si>
+    <t>cDocenteUbigeo</t>
+  </si>
+  <si>
+    <t>dDocenteFechaNacimiento</t>
+  </si>
+  <si>
+    <t>cDocenteDireccion</t>
+  </si>
+  <si>
+    <t>cDocenteTelefono</t>
+  </si>
+  <si>
+    <t>v_cDocenteTelefono</t>
+  </si>
+  <si>
+    <t>iHorasLabora</t>
+  </si>
+  <si>
+    <t>v_iHorasLabora</t>
+  </si>
+  <si>
+    <t>iPersCargoId</t>
+  </si>
+  <si>
+    <t>v_iPersCargoId</t>
+  </si>
+  <si>
+    <t>json_excel</t>
+  </si>
+  <si>
+    <t>lista_no_d</t>
   </si>
 </sst>
 </file>
@@ -116,11 +195,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,119 +481,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T27"/>
+  <dimension ref="A1:Y28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C27"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="T1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>27440013</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>70000000</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>70000000</v>
-      </c>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>70000001</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>70000002</v>
+        <v>70000001</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>70000003</v>
+        <v>70000002</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -521,9 +673,9 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>70000004</v>
+        <v>70000003</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -533,9 +685,9 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>70000005</v>
+        <v>70000004</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -545,9 +697,9 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>70000006</v>
+        <v>70000005</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -556,9 +708,9 @@
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>70000007</v>
+        <v>70000006</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -568,9 +720,9 @@
       <c r="S10" s="2"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>70000008</v>
+        <v>70000007</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -580,9 +732,9 @@
       <c r="S11" s="2"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>70000009</v>
+        <v>70000008</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -592,9 +744,9 @@
       <c r="S12" s="2"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>70000010</v>
+        <v>70000009</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -604,9 +756,9 @@
       <c r="S13" s="2"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>70000011</v>
+        <v>70000010</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -616,9 +768,9 @@
       <c r="S14" s="2"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>70000012</v>
+        <v>70000011</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -628,9 +780,9 @@
       <c r="S15" s="2"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>70000013</v>
+        <v>70000012</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -642,7 +794,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>70000014</v>
+        <v>70000013</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -654,10 +806,10 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>70000015</v>
+        <v>70000014</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="C18" s="4"/>
       <c r="O18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -666,7 +818,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>70000016</v>
+        <v>70000015</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -678,7 +830,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>70000017</v>
+        <v>70000016</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -690,7 +842,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>70000018</v>
+        <v>70000017</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -702,7 +854,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>70000019</v>
+        <v>70000018</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -714,7 +866,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>70000020</v>
+        <v>70000019</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -726,7 +878,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>70000021</v>
+        <v>70000020</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -737,7 +889,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>70000022</v>
+        <v>70000021</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -748,7 +900,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>70000023</v>
+        <v>70000022</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -756,14 +908,186 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>70000024</v>
+        <v>70000023</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>70000024</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ABAC64-CFFC-4585-8FA7-93CE8EC81BCD}">
+  <dimension ref="A1:Y2"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:Y2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" t="s">
+        <v>37</v>
+      </c>
+      <c r="W2" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Renombrar métodos de validación y agregar nuevas rutas para la validación de docentes y estudiantes
</commit_message>
<xml_diff>
--- a/storage/templates/import/bulk-data/plantilla-docente.xlsx
+++ b/storage/templates/import/bulk-data/plantilla-docente.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Projects\PyEduVirtual\PyEducaVirtualBackend\storage\templates\import\bulk-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096F91CF-28AF-4B04-A8D4-F3FD3E482E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80665A3B-D684-4F83-974B-6B400305357C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>DNI</t>
   </si>
@@ -195,12 +195,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,441 +480,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y28"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>27440013</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>27440013</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>70000000</v>
       </c>
+      <c r="B3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>70000001</v>
+      </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>70000001</v>
+        <v>70000002</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I5" s="2"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>70000002</v>
+        <v>70000003</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>70000003</v>
+        <v>70000004</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>70000004</v>
+        <v>70000005</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I8" s="2"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>70000005</v>
+        <v>70000006</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>70000006</v>
+        <v>70000007</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="3"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>70000007</v>
+        <v>70000008</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="3"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>70000008</v>
+        <v>70000009</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="3"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>70000009</v>
+        <v>70000010</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="3"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>70000010</v>
+        <v>70000011</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="3"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>70000011</v>
+        <v>70000012</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="3"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>70000012</v>
+        <v>70000013</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="3"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>70000013</v>
+        <v>70000014</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="3"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>70000014</v>
+        <v>70000015</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="4"/>
-      <c r="O18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="3"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>70000015</v>
+        <v>70000016</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="3"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>70000016</v>
+        <v>70000017</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="3"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>70000017</v>
+        <v>70000018</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="3"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>70000018</v>
+        <v>70000019</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="3"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>70000019</v>
+        <v>70000020</v>
       </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="3"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>70000020</v>
+        <v>70000021</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>70000021</v>
+        <v>70000022</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>70000022</v>
+        <v>70000023</v>
       </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="O26" s="2"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>70000023</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="O27" s="2"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
         <v>70000024</v>
       </c>
     </row>

</xml_diff>